<commit_message>
updating requirements and pandas basics
</commit_message>
<xml_diff>
--- a/weather_data.xlsx
+++ b/weather_data.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="weather" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="nans" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,308 +434,267 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>day</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>temperature</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>windspeed</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>event</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>1/1/2017</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>32</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Rain</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>1/4/2017</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>not available</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Sunny</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>1/5/2017</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>not measured</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Snow</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>1/6/2017</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>not available</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>no event</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>1/7/2017</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>not measured</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>32</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Rain</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>1/8/2017</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>not available</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>not measured</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
         <is>
           <t>Sunny</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>1/9/2017</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>not available</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>not measured</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>no event</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>1/10/2017</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>34</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>Cloudy</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>1/11/2017</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>-4</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
+      <c r="C10" t="n">
+        <v>-4</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
         <is>
           <t>Snow</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>1/12/2017</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
+      <c r="C11" t="n">
+        <v>26</v>
+      </c>
+      <c r="D11" t="n">
+        <v>12</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>Sunny</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>1/13/2017</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="C12" t="n">
+        <v>12</v>
+      </c>
+      <c r="D12" t="n">
+        <v>12</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>Rainy</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>1/11/2017</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
+      <c r="C13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>Snow</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>1/14/2017</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
+      <c r="C14" t="n">
+        <v>40</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
         <is>
           <t>Sunny</t>
         </is>

</xml_diff>